<commit_message>
modified:   android/app/src/main/AndroidManifest.xml 	modified:   assets/form/TOUKZ.xlsx 	new file:   assets/form/TOUPZ.xlsx 	new file:   assets/ukz.jpg 	modified:   lib/auth.dart 	new file:   lib/dbhelper_upz.dart 	modified:   lib/load_prog.dart 	new file:   lib/model_upz.dart 	modified:   lib/object_detail_ukz.dart 	new file:   lib/object_detail_upz.dart 	modified:   lib/object_list_ukz.dart 	new file:   lib/object_list_upz.dart 	modified:   lib/start_page.dart 	modified:   pubspec.yaml
</commit_message>
<xml_diff>
--- a/assets/form/TOUKZ.xlsx
+++ b/assets/form/TOUKZ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\flutterDartProjects\ehz1\assets\form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8DAC8A-AC3C-4D3A-B0E2-6C76E7BAF7C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AFB70D-07AC-4CFA-90D4-FC577BA3DC76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DAF5858F-70BD-47AC-AD03-F61C552FF57C}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="75">
-  <si>
-    <t>Протокол обслуживания УКЗ №____</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="74">
   <si>
     <t>"____"___________ 20____г.</t>
   </si>
@@ -657,12 +654,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="8">
@@ -758,7 +761,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -786,15 +789,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -807,6 +801,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1123,7 +1127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F5DDDF-532E-40E3-8C7B-62E63B846C9A}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -1144,562 +1148,560 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+    </row>
+    <row r="2" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-    </row>
-    <row r="2" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+    </row>
+    <row r="3" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-    </row>
-    <row r="3" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="17"/>
+      <c r="E3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13" t="s">
+      <c r="F3" s="17"/>
+      <c r="G3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="17"/>
+      <c r="I3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13" t="s">
+      <c r="J3" s="17"/>
+      <c r="K3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="L3" s="13"/>
+      <c r="L3" s="17"/>
     </row>
     <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="18" t="s">
         <v>16</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
         <v>18</v>
-      </c>
-      <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>29</v>
+      <c r="A9" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L9" s="10"/>
     </row>
     <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="18" t="s">
         <v>35</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="18" t="s">
         <v>40</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="13" t="s">
+      <c r="D12" s="17"/>
+      <c r="E12" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13" t="s">
+      <c r="F12" s="17"/>
+      <c r="G12" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="17"/>
+      <c r="I12" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L12" s="10"/>
     </row>
     <row r="13" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L15" s="10"/>
     </row>
     <row r="16" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L18" s="10"/>
     </row>
     <row r="19" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="18" t="s">
         <v>35</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="18" t="s">
         <v>40</v>
-      </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
     </row>
     <row r="25" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
@@ -1717,19 +1719,14 @@
     </row>
     <row r="26" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E26" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="A21:L21"/>
-    <mergeCell ref="A22:L22"/>
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="A24:L24"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:L2"/>
@@ -1744,8 +1741,13 @@
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="A22:L22"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="A24:L24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="55" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="55" orientation="landscape" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new file:   assets/form/TOUDZ.xlsx 	modified:   assets/form/TOUKZ.xlsx 	modified:   assets/form/TOUPZ.xlsx 	new file:   lib/dbhelper_udz.dart 	new file:   lib/model_udz.dart 	modified:   lib/model_upz.dart 	modified:   lib/object_detail_upz.dart 	modified:   lib/object_list_upz.dart
</commit_message>
<xml_diff>
--- a/assets/form/TOUKZ.xlsx
+++ b/assets/form/TOUKZ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\flutterDartProjects\ehz1\assets\form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AFB70D-07AC-4CFA-90D4-FC577BA3DC76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C1E3E9-DA3C-4369-A1F1-F0351C52569D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DAF5858F-70BD-47AC-AD03-F61C552FF57C}"/>
   </bookViews>
@@ -533,6 +533,57 @@
     <t>Катодная линия</t>
   </si>
   <si>
+    <t>Сопротивление растеканию анода №4, Ом</t>
+  </si>
+  <si>
+    <t>Состояние катодной ВЛ</t>
+  </si>
+  <si>
+    <t>Сопротивление цепи СКЗ, Ом</t>
+  </si>
+  <si>
+    <t>Удельное сопротивление  грунта в районе АЗ, Ом*м</t>
+  </si>
+  <si>
+    <t>Состояние катодной КЛ</t>
+  </si>
+  <si>
+    <t>Эл.счётчик. кВт*ч</t>
+  </si>
+  <si>
+    <t>Удельное сопротивление  грунта в районе КТП, Ом*м</t>
+  </si>
+  <si>
+    <t>Другое</t>
+  </si>
+  <si>
+    <t>Счётчик наработки, ч</t>
+  </si>
+  <si>
+    <t>Удельное сопротивление грунта в районе разъединителя, Ом*м</t>
+  </si>
+  <si>
+    <t>Состояние ограждения</t>
+  </si>
+  <si>
+    <t>Счётчик защиты, ч</t>
+  </si>
+  <si>
+    <t>Состояние территории</t>
+  </si>
+  <si>
+    <t>Замечания</t>
+  </si>
+  <si>
+    <t>(ФИО)</t>
+  </si>
+  <si>
+    <t>Подпись</t>
+  </si>
+  <si>
+    <t>БДР №2</t>
+  </si>
+  <si>
     <r>
       <t>Напряжение на шунте</t>
     </r>
@@ -552,61 +603,12 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> В</t>
-    </r>
-  </si>
-  <si>
-    <t>Сопротивление растеканию анода №4, Ом</t>
-  </si>
-  <si>
-    <t>Состояние катодной ВЛ</t>
-  </si>
-  <si>
-    <t>Сопротивление цепи СКЗ, Ом</t>
-  </si>
-  <si>
-    <t>Удельное сопротивление  грунта в районе АЗ, Ом*м</t>
-  </si>
-  <si>
-    <t>Состояние катодной КЛ</t>
-  </si>
-  <si>
-    <t>Эл.счётчик. кВт*ч</t>
-  </si>
-  <si>
-    <t>Удельное сопротивление  грунта в районе КТП, Ом*м</t>
-  </si>
-  <si>
-    <t>Другое</t>
-  </si>
-  <si>
-    <t>Счётчик наработки, ч</t>
-  </si>
-  <si>
-    <t>Удельное сопротивление грунта в районе разъединителя, Ом*м</t>
-  </si>
-  <si>
-    <t>Состояние ограждения</t>
-  </si>
-  <si>
-    <t>Счётчик защиты, ч</t>
-  </si>
-  <si>
-    <t>Состояние территории</t>
-  </si>
-  <si>
-    <t>Замечания</t>
-  </si>
-  <si>
-    <t>(ФИО)</t>
-  </si>
-  <si>
-    <t>Подпись</t>
-  </si>
-  <si>
-    <t>БДР №2</t>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> мВ</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -761,7 +763,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -783,10 +785,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -801,16 +813,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1127,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F5DDDF-532E-40E3-8C7B-62E63B846C9A}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,60 +1151,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
+      <c r="A1" s="12"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
     </row>
     <row r="2" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
     </row>
     <row r="3" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17" t="s">
+      <c r="H3" s="14"/>
+      <c r="I3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17" t="s">
+      <c r="J3" s="14"/>
+      <c r="K3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="17"/>
+      <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1272,7 +1275,7 @@
         <v>15</v>
       </c>
       <c r="H6" s="2"/>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="9" t="s">
         <v>16</v>
       </c>
       <c r="J6" s="2"/>
@@ -1282,7 +1285,7 @@
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="2"/>
@@ -1336,7 +1339,7 @@
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="2"/>
@@ -1356,10 +1359,10 @@
         <v>31</v>
       </c>
       <c r="J9" s="2"/>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="L9" s="10"/>
+      <c r="L9" s="11"/>
     </row>
     <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1374,7 +1377,7 @@
         <v>34</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="9" t="s">
         <v>35</v>
       </c>
       <c r="H10" s="2"/>
@@ -1400,7 +1403,7 @@
         <v>39</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="9" t="s">
         <v>40</v>
       </c>
       <c r="H11" s="2"/>
@@ -1414,30 +1417,30 @@
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17" t="s">
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="H12" s="17"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="14"/>
       <c r="I12" s="3" t="s">
         <v>46</v>
       </c>
       <c r="J12" s="2"/>
-      <c r="K12" s="9" t="s">
+      <c r="K12" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="L12" s="10"/>
+      <c r="L12" s="11"/>
     </row>
     <row r="13" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1492,7 +1495,7 @@
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="19" t="s">
         <v>35</v>
       </c>
       <c r="B15" s="2"/>
@@ -1512,14 +1515,14 @@
         <v>54</v>
       </c>
       <c r="J15" s="2"/>
-      <c r="K15" s="9" t="s">
+      <c r="K15" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="L15" s="10"/>
+      <c r="L15" s="11"/>
     </row>
     <row r="16" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>56</v>
+      <c r="A16" s="19" t="s">
+        <v>73</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="1" t="s">
@@ -1535,17 +1538,17 @@
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="1" t="s">
@@ -1561,17 +1564,17 @@
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="1" t="s">
@@ -1587,17 +1590,17 @@
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="L18" s="10"/>
+      <c r="L18" s="11"/>
     </row>
     <row r="19" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="1" t="s">
@@ -1608,22 +1611,22 @@
         <v>34</v>
       </c>
       <c r="F19" s="2"/>
-      <c r="G19" s="18" t="s">
+      <c r="G19" s="9" t="s">
         <v>35</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="1" t="s">
@@ -1634,74 +1637,74 @@
         <v>39</v>
       </c>
       <c r="F20" s="2"/>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="9" t="s">
         <v>40</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
     </row>
     <row r="25" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
@@ -1719,14 +1722,19 @@
     </row>
     <row r="26" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E26" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G26" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="A22:L22"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="A24:L24"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:L2"/>
@@ -1741,11 +1749,6 @@
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="A21:L21"/>
-    <mergeCell ref="A22:L22"/>
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="A24:L24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="55" orientation="landscape" verticalDpi="1200" r:id="rId1"/>

</xml_diff>